<commit_message>
Removed unnecessary "Randomizer" file. Created an initial stat generator for Members
</commit_message>
<xml_diff>
--- a/Data/Band_Sim_Vars_V1.xlsx
+++ b/Data/Band_Sim_Vars_V1.xlsx
@@ -19,12 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="127">
-  <si>
-    <t>Electric Guitar</t>
-  </si>
-  <si>
-    <t>Acoustic Guitar</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="111">
+  <si>
+    <t>Guitar</t>
   </si>
   <si>
     <t>Bass</t>
@@ -33,55 +30,10 @@
     <t>Drums</t>
   </si>
   <si>
-    <t>Piano</t>
-  </si>
-  <si>
-    <t>Synth</t>
-  </si>
-  <si>
-    <t>Trumpet</t>
-  </si>
-  <si>
-    <t>Saxophone</t>
-  </si>
-  <si>
-    <t>Flute</t>
-  </si>
-  <si>
-    <t>Violin</t>
-  </si>
-  <si>
-    <t>Cello</t>
-  </si>
-  <si>
-    <t>Cowbell</t>
-  </si>
-  <si>
-    <t>Triangle</t>
-  </si>
-  <si>
-    <t>Tamborine</t>
-  </si>
-  <si>
-    <t>Harp</t>
-  </si>
-  <si>
-    <t>Banjo</t>
-  </si>
-  <si>
-    <t>Harmonica</t>
-  </si>
-  <si>
-    <t>Bongos</t>
+    <t>Keyboard</t>
   </si>
   <si>
     <t>Vocals</t>
-  </si>
-  <si>
-    <t>Theremin</t>
-  </si>
-  <si>
-    <t>Trombone</t>
   </si>
   <si>
     <t>Rock</t>
@@ -713,86 +665,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -810,82 +682,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -908,127 +780,127 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1051,47 +923,47 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1111,82 +983,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1206,82 +1078,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1301,82 +1173,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1396,32 +1268,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1441,22 +1313,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the Make Album menu to have genre and album type dropdowns. Added a Make Album button, but there's no functionality yet. Created Album Types sheet in vars doc
</commit_message>
<xml_diff>
--- a/Data/Band_Sim_Vars_V1.xlsx
+++ b/Data/Band_Sim_Vars_V1.xlsx
@@ -5,13 +5,14 @@
   <sheets>
     <sheet state="visible" name="Instrument" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Genre" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="First Name" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Last Name" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Band1" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="Band2" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="Band3" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="Location Name" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="Location Type" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="Album Type" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="First Name" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Last Name" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="Band1" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="Band2" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="Band3" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="Location Name" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="Location Type" sheetId="10" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="114">
   <si>
     <t>Guitar</t>
   </si>
@@ -82,6 +83,15 @@
   </si>
   <si>
     <t>A capella</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>DVD</t>
+  </si>
+  <si>
+    <t>Vinyl</t>
   </si>
   <si>
     <t>John</t>
@@ -401,6 +411,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -670,6 +684,41 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -766,6 +815,45 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -780,127 +868,127 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -908,7 +996,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -923,142 +1011,47 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1078,82 +1071,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1173,82 +1166,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1268,32 +1261,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>106</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1313,22 +1356,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>107</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>109</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added better name generation. Bands and Albums will append an 's' to the end of a plural
</commit_message>
<xml_diff>
--- a/Data/Band_Sim_Vars_V1.xlsx
+++ b/Data/Band_Sim_Vars_V1.xlsx
@@ -1098,40 +1098,64 @@
       <c r="A6" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="B6" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="B7" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="B8" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="B9" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="B10" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="B11" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="B12" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
         <v>70</v>
+      </c>
+      <c r="B13" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="14">

</xml_diff>